<commit_message>
Added initial plots and transformed data a bit, need to split the plots up so that they are on separate plots.
</commit_message>
<xml_diff>
--- a/CPIDataCleaned.xlsx
+++ b/CPIDataCleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Zhu-Daniel.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daniel_Zhu_Account/Documents/Zhu-Daniel.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D986498E-0211-4487-986D-948D156E4A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C22C1D3-ECC7-854C-9F13-1360AE6BDCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B1852B38-DDFB-47C2-85D4-2D4B01159D02}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{B1852B38-DDFB-47C2-85D4-2D4B01159D02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,8 +113,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -367,31 +367,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="10"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="11"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -400,64 +400,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="13"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
@@ -779,12 +779,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.578125" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:48" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +930,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>5</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>8</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>15</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>16</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>18</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>20</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>21</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>22</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:48" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:48" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>23</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="24" spans="1:48" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="1:48" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>